<commit_message>
Bulk changes and improvements for loading footings file and asserting equal.
</commit_message>
<xml_diff>
--- a/tests/data/expected-footings-wb.xlsx
+++ b/tests/data/expected-footings-wb.xlsx
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1455,7 +1455,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[key]</t>
+          <t>/key/</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[('tuple', 'key')]</t>
+          <t>/('tuple', 'key')/</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[('tuple', 'key')]</t>
+          <t>/('tuple', 'key')/</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[a]</t>
+          <t>/a/</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[a]</t>
+          <t>/a/</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[b]</t>
+          <t>/b/</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[b]</t>
+          <t>/b/</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[a]</t>
+          <t>/a/</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[a]</t>
+          <t>/a/</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[b]</t>
+          <t>/b/</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[b]</t>
+          <t>/b/</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">

</xml_diff>

<commit_message>
Refactored to_json for ErrorCatch and added capabilties for to_xlsx.
</commit_message>
<xml_diff>
--- a/tests/data/expected-footings-wb.xlsx
+++ b/tests/data/expected-footings-wb.xlsx
@@ -14,7 +14,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test-iterable" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test-custom" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test-function" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="__footings__" sheetId="8" state="hidden" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test-error-catch" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="__footings__" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -944,7 +945,74 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="B2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>key</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'k1': '1'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>error_type</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TypeError</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>error_value</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>("__init__() missing 1 required keyword-only argument: 'k2'",)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>error_stacktrace</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['  File "/home/dustintindall/anaconda3/lib/python3.7/site-packages/footings/parallel_tools/base.py", line 107, in wrapper\n    ret = model(**model_kwargs).run()\n']</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2459,6 +2527,278 @@
         <v>2</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>/key/</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>2</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2</v>
+      </c>
+      <c r="K52" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>/key/</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>3</v>
+      </c>
+      <c r="J53" t="n">
+        <v>2</v>
+      </c>
+      <c r="K53" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>/error_type/</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>3</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2</v>
+      </c>
+      <c r="J54" t="n">
+        <v>3</v>
+      </c>
+      <c r="K54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>/error_type/</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" t="n">
+        <v>3</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3</v>
+      </c>
+      <c r="K55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>/error_value/</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>4</v>
+      </c>
+      <c r="I56" t="n">
+        <v>2</v>
+      </c>
+      <c r="J56" t="n">
+        <v>4</v>
+      </c>
+      <c r="K56" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>/error_value/</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>4</v>
+      </c>
+      <c r="I57" t="n">
+        <v>3</v>
+      </c>
+      <c r="J57" t="n">
+        <v>4</v>
+      </c>
+      <c r="K57" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>/error_stacktrace/</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>KEY</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>5</v>
+      </c>
+      <c r="I58" t="n">
+        <v>2</v>
+      </c>
+      <c r="J58" t="n">
+        <v>5</v>
+      </c>
+      <c r="K58" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>test-error-catch</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>/error_stacktrace/</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>5</v>
+      </c>
+      <c r="I59" t="n">
+        <v>3</v>
+      </c>
+      <c r="J59" t="n">
+        <v>5</v>
+      </c>
+      <c r="K59" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Set error_stacktrace to [] given it was generating dynamic content based on line number.
</commit_message>
<xml_diff>
--- a/tests/data/expected-footings-wb.xlsx
+++ b/tests/data/expected-footings-wb.xlsx
@@ -99,7 +99,7 @@
     <t xml:space="preserve">error_stacktrace</t>
   </si>
   <si>
-    <t xml:space="preserve">['  File "/home/dustintindall/anaconda3/lib/python3.7/site-packages/footings/parallel_tools/base.py", line 108, in wrapper\n    ret = model(**model_kwargs).run()\n']</t>
+    <t xml:space="preserve">[]</t>
   </si>
   <si>
     <t xml:space="preserve">worksheet</t>
@@ -279,8 +279,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,56 +316,56 @@
   <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>1.23456789</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>43465</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>43465.5</v>
       </c>
     </row>
@@ -384,48 +388,48 @@
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -448,32 +452,32 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -496,74 +500,74 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" s="0" t="s">
+      <c r="C11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -586,101 +590,101 @@
   <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -703,40 +707,40 @@
   <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -759,13 +763,13 @@
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -788,40 +792,40 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:C5"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -844,1401 +848,1401 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:C5 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" s="0" t="n">
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" s="0" t="n">
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" s="0" t="n">
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="I6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="I7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" s="0" t="n">
+      <c r="I8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I9" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" s="0" t="n">
+      <c r="I9" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="0" t="n">
+      <c r="F10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="0" t="n">
+      <c r="I10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J11" s="0" t="n">
+      <c r="I11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="0" t="n">
+      <c r="F12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="0" t="n">
+      <c r="I12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J13" s="0" t="n">
+      <c r="I13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="0" t="n">
+      <c r="H14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I15" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="0" t="n">
+      <c r="I15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="0" t="n">
+      <c r="H16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J17" s="0" t="n">
+      <c r="H17" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K18" s="0" t="n">
+      <c r="F18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K19" s="0" t="n">
+      <c r="F19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="0" t="n">
+      <c r="F20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I20" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J20" s="0" t="n">
+      <c r="I20" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J21" s="0" t="n">
+      <c r="I21" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J22" s="0" t="n">
+      <c r="I22" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I23" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J23" s="0" t="n">
+      <c r="I23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I24" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J24" s="0" t="n">
+      <c r="I24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="0" t="n">
+      <c r="F25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="I25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J25" s="0" t="n">
+      <c r="I25" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="I26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J26" s="0" t="n">
+      <c r="I26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="F27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="J27" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="0" t="n">
+      <c r="F28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="I28" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J28" s="0" t="n">
+      <c r="I28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="K28" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="F29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="I29" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J29" s="0" t="n">
+      <c r="I29" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J29" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="K29" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K30" s="0" t="n">
+      <c r="H30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K30" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K31" s="0" t="n">
+      <c r="H31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K31" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="0" t="s">
+      <c r="F32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I32" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J32" s="0" t="n">
+      <c r="I32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J32" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="K32" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F33" s="0" t="s">
+      <c r="F33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I33" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J33" s="0" t="n">
+      <c r="I33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K33" s="0" t="n">
+      <c r="K33" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="0" t="s">
+      <c r="F34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I34" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J34" s="0" t="n">
+      <c r="I34" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J34" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="K34" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="F35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="I35" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J35" s="0" t="n">
+      <c r="I35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K35" s="0" t="n">
+      <c r="K35" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="0" t="s">
+      <c r="F36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J36" s="0" t="n">
+      <c r="I36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J36" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K36" s="0" t="n">
+      <c r="K36" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="0" t="s">
+      <c r="F37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="I37" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J37" s="0" t="n">
+      <c r="I37" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J37" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="K37" s="0" t="n">
+      <c r="K37" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F38" s="0" t="s">
+      <c r="F38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="I38" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J38" s="0" t="n">
+      <c r="I38" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J38" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="K38" s="0" t="n">
+      <c r="K38" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="0" t="s">
+      <c r="F39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="I39" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J39" s="0" t="n">
+      <c r="I39" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J39" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K39" s="0" t="n">
+      <c r="K39" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="I40" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J40" s="0" t="n">
+      <c r="I40" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J40" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="K40" s="0" t="n">
+      <c r="K40" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="0" t="s">
+      <c r="F41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="I41" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J41" s="0" t="n">
+      <c r="I41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J41" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="K41" s="0" t="n">
+      <c r="K41" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="I42" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J42" s="0" t="n">
+      <c r="I42" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J42" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="K42" s="0" t="n">
+      <c r="K42" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H43" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I43" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J43" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K43" s="0" t="n">
+      <c r="F43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K43" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K44" s="0" t="n">
+      <c r="H44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K44" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F45" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H45" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J45" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K45" s="0" t="n">
+      <c r="F45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K45" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="F46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H46" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J46" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K46" s="0" t="n">
+      <c r="H46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K46" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F47" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H47" s="0" t="n">
+      <c r="F47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H47" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I47" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J47" s="0" t="n">
+      <c r="I47" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J47" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K47" s="0" t="n">
+      <c r="K47" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F48" s="0" t="s">
+      <c r="F48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="H48" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I48" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J48" s="0" t="n">
+      <c r="I48" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J48" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K48" s="0" t="n">
+      <c r="K48" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F49" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H49" s="0" t="n">
+      <c r="F49" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I49" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J49" s="0" t="n">
+      <c r="I49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J49" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K49" s="0" t="n">
+      <c r="K49" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F50" s="0" t="s">
+      <c r="F50" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="H50" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I50" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J50" s="0" t="n">
+      <c r="I50" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J50" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K50" s="0" t="n">
+      <c r="K50" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F51" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H51" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I51" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J51" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K51" s="0" t="n">
+      <c r="F51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J51" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K51" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F52" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H52" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I52" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J52" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K52" s="0" t="n">
+      <c r="F52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K52" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H53" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="I53" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J53" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K53" s="0" t="n">
+      <c r="F53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K53" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F54" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H54" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I54" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J54" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K54" s="0" t="n">
+      <c r="F54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K54" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F55" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H55" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I55" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J55" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="K55" s="0" t="n">
+      <c r="F55" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J55" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K55" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F56" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H56" s="0" t="n">
+      <c r="F56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H56" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I56" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J56" s="0" t="n">
+      <c r="I56" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J56" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K56" s="0" t="n">
+      <c r="K56" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F57" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H57" s="0" t="n">
+      <c r="F57" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H57" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I57" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J57" s="0" t="n">
+      <c r="I57" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J57" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="K57" s="0" t="n">
+      <c r="K57" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F58" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H58" s="0" t="n">
+      <c r="F58" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H58" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I58" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J58" s="0" t="n">
+      <c r="I58" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J58" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K58" s="0" t="n">
+      <c r="K58" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F59" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H59" s="0" t="n">
+      <c r="F59" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I59" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J59" s="0" t="n">
+      <c r="I59" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J59" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K59" s="0" t="n">
+      <c r="K59" s="1" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>